<commit_message>
Validación final (prev 2022 para DM y ERC)
</commit_message>
<xml_diff>
--- a/dat/validacion.xlsx
+++ b/dat/validacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zulmacucunuba/Documents/GIT/quality-rips-surveillance/dat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5f934af0bcd737c/Documentos/DanielaBM/2023/3. Trabajo/Asistente investigativo PUJ/quality-rips-surveillance/quality-rips-surveillance/dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC972447-35E7-DF43-A9D9-375FC59711E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{EC972447-35E7-DF43-A9D9-375FC59711E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F17ABFA7-0F59-48FE-A184-F152A8F0A02D}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{2E6F7CA9-190C-2745-AC5C-30693F336DBA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2E6F7CA9-190C-2745-AC5C-30693F336DBA}"/>
   </bookViews>
   <sheets>
     <sheet name="prevalencias" sheetId="1" r:id="rId1"/>
@@ -36,43 +36,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>enfermedad</t>
   </si>
   <si>
-    <t>Diabetes Mellitus</t>
-  </si>
-  <si>
     <t>prevalencia</t>
   </si>
   <si>
     <t>ref</t>
   </si>
   <si>
-    <t>0.10</t>
-  </si>
-  <si>
-    <t>Rosselli et al 2020</t>
-  </si>
-  <si>
     <t>ref_link</t>
   </si>
   <si>
-    <t>wwww.ññññññ</t>
-  </si>
-  <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>0.0312</t>
+  </si>
+  <si>
+    <t>https://cuentadealtocosto.org/wp-content/uploads/2023/10/final-libro-erc-2022-2.pdf</t>
+  </si>
+  <si>
+    <t>0.0154</t>
+  </si>
+  <si>
+    <t>Fondo Colombiano de Enfermedades de Alto Costo. Situación de la enfermedad renal crónica, la hipertensión arterial y la diabetes mellitus en Colombia 2022. Colombia: CAC; 2023. Pag. 54</t>
+  </si>
+  <si>
+    <t>Fondo Colombiano de Enfermedades de Alto Costo. Situación de la enfermedad renal crónica, la hipertensión arterial y la diabetes mellitus en Colombia 2022. Colombia: CAC; 2023. Pag. 67</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>ERC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,16 +112,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -120,8 +140,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -417,13 +441,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269C429F-CDA3-424C-B82E-F824169333A5}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
@@ -431,41 +455,62 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2020</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{73956DA5-4932-48FD-97BF-7D91E8491584}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{7DBFBE1D-F08F-492C-B32D-00A0200E3D45}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>